<commit_message>
Se agregó nombre y puesto de trabajo de Alvaro Alburez.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git2021\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE6BE09-5536-4324-9838-0D9F767D1B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1A9B95-3978-45CD-86A8-140F1E3E44FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t xml:space="preserve">Progamador#1: Base de datos </t>
+  </si>
+  <si>
+    <t>Alvaro Ramiro Alburez Rivera</t>
+  </si>
+  <si>
+    <t>Progamador#2</t>
   </si>
 </sst>
 </file>
@@ -318,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,28 +333,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -364,6 +355,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,12 +689,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -707,47 +713,47 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -766,62 +772,66 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="15" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="9" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="5"/>
@@ -831,16 +841,16 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
@@ -850,16 +860,16 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5"/>
@@ -869,16 +879,16 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
@@ -888,16 +898,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -907,16 +917,16 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -926,16 +936,16 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -945,16 +955,16 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="12"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -964,16 +974,16 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -983,16 +993,16 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
@@ -1002,7 +1012,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1021,7 +1031,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1040,7 +1050,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1059,7 +1069,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1078,7 +1088,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1097,7 +1107,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1116,7 +1126,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1135,7 +1145,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1154,7 +1164,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1173,7 +1183,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1192,7 +1202,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1211,7 +1221,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1230,7 +1240,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1249,7 +1259,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1268,7 +1278,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1287,7 +1297,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1306,7 +1316,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1325,7 +1335,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1344,7 +1354,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1363,7 +1373,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1382,7 +1392,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1401,7 +1411,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1420,7 +1430,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1439,7 +1449,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1458,7 +1468,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1477,7 +1487,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1496,7 +1506,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1515,7 +1525,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1534,7 +1544,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1553,7 +1563,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1572,7 +1582,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1591,7 +1601,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1610,7 +1620,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1629,7 +1639,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1648,7 +1658,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1667,7 +1677,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1686,7 +1696,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1705,7 +1715,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1724,7 +1734,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1743,7 +1753,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1762,7 +1772,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1781,7 +1791,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1800,7 +1810,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1819,7 +1829,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1838,7 +1848,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1857,7 +1867,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1876,7 +1886,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1895,7 +1905,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1914,7 +1924,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1933,7 +1943,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1952,7 +1962,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1971,7 +1981,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1990,7 +2000,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2009,7 +2019,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2028,7 +2038,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2047,7 +2057,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2066,7 +2076,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2085,7 +2095,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2106,6 +2116,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2122,15 +2141,6 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Josue Alvarado.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git2021\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1A9B95-3978-45CD-86A8-140F1E3E44FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B568E-E76D-4BAA-9484-424ABCC132FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Progamador#2</t>
+  </si>
+  <si>
+    <t>Josue Daniel Alvarado Cabrera</t>
+  </si>
+  <si>
+    <t>Programador #3</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -333,13 +339,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -363,13 +375,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,12 +695,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I8" sqref="I8:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -713,47 +719,47 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -772,64 +778,64 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="17" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="4"/>
@@ -841,16 +847,20 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="16"/>
+      <c r="I8" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
@@ -860,16 +870,16 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="16"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5"/>
@@ -879,16 +889,16 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="16"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
@@ -898,16 +908,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="16"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -917,16 +927,16 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="16"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -936,16 +946,16 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="16"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -955,16 +965,16 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="16"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -974,16 +984,16 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -993,16 +1003,16 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="18"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
@@ -1012,7 +1022,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1031,7 +1041,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1050,7 +1060,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1069,7 +1079,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1088,7 +1098,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1107,7 +1117,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1126,7 +1136,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1145,7 +1155,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1164,7 +1174,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1183,7 +1193,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1202,7 +1212,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1221,7 +1231,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1240,7 +1250,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1259,7 +1269,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1278,7 +1288,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1297,7 +1307,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1316,7 +1326,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1335,7 +1345,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1354,7 +1364,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1373,7 +1383,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1392,7 +1402,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1411,7 +1421,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1430,7 +1440,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1449,7 +1459,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1468,7 +1478,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1487,7 +1497,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1506,7 +1516,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1525,7 +1535,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1544,7 +1554,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1563,7 +1573,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1582,7 +1592,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1601,7 +1611,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1620,7 +1630,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1639,7 +1649,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1658,7 +1668,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1677,7 +1687,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1696,7 +1706,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1715,7 +1725,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1734,7 +1744,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1753,7 +1763,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1772,7 +1782,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1791,7 +1801,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1810,7 +1820,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1829,7 +1839,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1848,7 +1858,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1867,7 +1877,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1886,7 +1896,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1905,7 +1915,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1924,7 +1934,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1943,7 +1953,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1962,7 +1972,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1981,7 +1991,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2000,7 +2010,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2019,7 +2029,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2038,7 +2048,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2057,7 +2067,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2076,7 +2086,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2095,7 +2105,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2116,15 +2126,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2141,6 +2142,15 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Kikab Balan.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git2021\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B568E-E76D-4BAA-9484-424ABCC132FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98018B59-7531-4C90-8198-D1C7F54463D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Programador #3</t>
+  </si>
+  <si>
+    <t>Kikab Sergio Pablo Balan Velazco</t>
+  </si>
+  <si>
+    <t>Programador #4</t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -339,19 +345,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -375,7 +375,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -695,12 +701,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:L8"/>
+      <selection activeCell="I9" sqref="I9:L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -719,47 +725,47 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -778,64 +784,64 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="4"/>
@@ -847,18 +853,18 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="4"/>
@@ -870,16 +876,20 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5"/>
@@ -889,16 +899,16 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="9"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
@@ -908,16 +918,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -927,16 +937,16 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -946,16 +956,16 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -965,16 +975,16 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="9"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -984,16 +994,16 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="9"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -1003,16 +1013,16 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
@@ -1022,7 +1032,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1041,7 +1051,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1060,7 +1070,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1079,7 +1089,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1098,7 +1108,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1117,7 +1127,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1136,7 +1146,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1155,7 +1165,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1174,7 +1184,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1193,7 +1203,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1212,7 +1222,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1231,7 +1241,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1250,7 +1260,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1269,7 +1279,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1288,7 +1298,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1307,7 +1317,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1326,7 +1336,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1345,7 +1355,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1364,7 +1374,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1383,7 +1393,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1402,7 +1412,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1421,7 +1431,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1440,7 +1450,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1459,7 +1469,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1478,7 +1488,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1497,7 +1507,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1516,7 +1526,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1535,7 +1545,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1554,7 +1564,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1573,7 +1583,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1592,7 +1602,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1611,7 +1621,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1630,7 +1640,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1649,7 +1659,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1668,7 +1678,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1687,7 +1697,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1706,7 +1716,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1725,7 +1735,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1744,7 +1754,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1763,7 +1773,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1782,7 +1792,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1801,7 +1811,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1820,7 +1830,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1839,7 +1849,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1858,7 +1868,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1877,7 +1887,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1896,7 +1906,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1915,7 +1925,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1934,7 +1944,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1953,7 +1963,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1972,7 +1982,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1991,7 +2001,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2010,7 +2020,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2029,7 +2039,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2048,7 +2058,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2067,7 +2077,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2086,7 +2096,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2105,7 +2115,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2126,6 +2136,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2142,15 +2161,6 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Rodrigo Cárdenas.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git2021\ProyectoFinal_SneakersShoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98018B59-7531-4C90-8198-D1C7F54463D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFEC104-8A24-4281-B130-365FCC138B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Jacobo Efraín Ajquí Zunum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progamador#1: Base de datos </t>
   </si>
   <si>
     <t>Alvaro Ramiro Alburez Rivera</t>
@@ -58,6 +55,15 @@
   </si>
   <si>
     <t>Programador #4</t>
+  </si>
+  <si>
+    <t>Rodrigo Gerardo Cárdenas Monroy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progamador #1: Base de datos </t>
+  </si>
+  <si>
+    <t>Programador # 5: Modelo de Entidades</t>
   </si>
 </sst>
 </file>
@@ -336,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -345,13 +351,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -375,13 +387,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -701,12 +707,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:L9"/>
+      <selection activeCell="I10" sqref="I10:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -725,47 +731,47 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -784,65 +790,65 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="17" t="s">
-        <v>4</v>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18" t="s">
+        <v>11</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
+      <c r="E7" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="16" t="s">
-        <v>6</v>
+      <c r="I7" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -853,19 +859,19 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="16" t="s">
-        <v>8</v>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -876,19 +882,19 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
+      <c r="E9" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="16" t="s">
-        <v>10</v>
+      <c r="I9" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -899,16 +905,20 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="16"/>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
@@ -918,16 +928,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="16"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -937,16 +947,16 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="16"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -956,16 +966,16 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="16"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -975,16 +985,16 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="16"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -994,16 +1004,16 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -1013,16 +1023,16 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="18"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
@@ -1032,7 +1042,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1051,7 +1061,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1070,7 +1080,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1089,7 +1099,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1108,7 +1118,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1127,7 +1137,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1146,7 +1156,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1165,7 +1175,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1184,7 +1194,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1203,7 +1213,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1222,7 +1232,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1241,7 +1251,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1260,7 +1270,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1279,7 +1289,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1298,7 +1308,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1317,7 +1327,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1336,7 +1346,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1355,7 +1365,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1374,7 +1384,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1393,7 +1403,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1412,7 +1422,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1431,7 +1441,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1450,7 +1460,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1469,7 +1479,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1488,7 +1498,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1507,7 +1517,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1526,7 +1536,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1545,7 +1555,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1564,7 +1574,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1583,7 +1593,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1602,7 +1612,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1621,7 +1631,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1640,7 +1650,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1659,7 +1669,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1678,7 +1688,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1697,7 +1707,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1716,7 +1726,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1735,7 +1745,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1754,7 +1764,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1773,7 +1783,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1792,7 +1802,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1811,7 +1821,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1830,7 +1840,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1849,7 +1859,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1868,7 +1878,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1887,7 +1897,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1906,7 +1916,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1925,7 +1935,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1944,7 +1954,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1963,7 +1973,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1982,7 +1992,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2001,7 +2011,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2020,7 +2030,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2039,7 +2049,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2058,7 +2068,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2077,7 +2087,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2096,7 +2106,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2115,7 +2125,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2136,15 +2146,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2161,6 +2162,15 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Samuel Escobar.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFEC104-8A24-4281-B130-365FCC138B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F542BC76-095A-412D-B583-A27D1B052271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Programador # 5: Modelo de Entidades</t>
+  </si>
+  <si>
+    <t>Samuel Isaac Escobar Vásquez</t>
+  </si>
+  <si>
+    <t>Scrum Master</t>
   </si>
 </sst>
 </file>
@@ -342,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,19 +357,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -387,7 +387,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -707,7 +713,7 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:L10"/>
+      <selection activeCell="E12" sqref="E12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,16 +742,16 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -757,14 +763,14 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -795,18 +801,18 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -818,18 +824,18 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -841,13 +847,13 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="4"/>
@@ -864,13 +870,13 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="16" t="s">
         <v>7</v>
       </c>
       <c r="J8" s="4"/>
@@ -887,13 +893,13 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="4"/>
@@ -910,13 +916,13 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="4"/>
@@ -933,11 +939,15 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -952,11 +962,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -971,11 +981,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="5"/>
@@ -990,11 +1000,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="9"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -1009,11 +1019,11 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="9"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -1028,11 +1038,11 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
@@ -2146,6 +2156,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2162,15 +2181,6 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Sduard Ixpatac.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProyectoFinal_SneakersShoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git2021\ProyectoFinal_SneakersShop\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F542BC76-095A-412D-B583-A27D1B052271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A54D9FC-34B3-4E86-B19E-EEA645B7E361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -69,7 +69,13 @@
     <t>Samuel Isaac Escobar Vásquez</t>
   </si>
   <si>
-    <t>Scrum Master</t>
+    <t>Sduard Alejandro Ixpatac Sipaque</t>
+  </si>
+  <si>
+    <t>Scrum Master: Organización en Trello</t>
+  </si>
+  <si>
+    <t>Programador #9: Diagrama Entidad Relación</t>
   </si>
 </sst>
 </file>
@@ -344,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -396,6 +402,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,12 +720,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -737,7 +744,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -758,7 +765,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -777,7 +784,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -796,7 +803,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -819,7 +826,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -842,7 +849,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -865,7 +872,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -888,7 +895,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -911,7 +918,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -934,20 +941,16 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="I11" s="16"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -957,26 +960,30 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="19"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -995,7 +1002,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1014,16 +1021,20 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="5"/>
@@ -1033,7 +1044,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1052,7 +1063,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1071,7 +1082,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1090,7 +1101,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1109,7 +1120,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1128,7 +1139,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1147,7 +1158,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1166,7 +1177,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1185,7 +1196,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1204,7 +1215,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1223,7 +1234,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1242,7 +1253,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1261,7 +1272,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1280,7 +1291,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1299,7 +1310,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1318,7 +1329,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1337,7 +1348,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1356,7 +1367,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1375,7 +1386,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1394,7 +1405,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1413,7 +1424,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1432,7 +1443,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1451,7 +1462,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1470,7 +1481,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1489,7 +1500,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1508,7 +1519,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1527,7 +1538,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1546,7 +1557,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1565,7 +1576,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1584,7 +1595,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1603,7 +1614,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1622,7 +1633,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1641,7 +1652,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1660,7 +1671,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1679,7 +1690,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1698,7 +1709,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1717,7 +1728,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1736,7 +1747,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1755,7 +1766,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1774,7 +1785,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1793,7 +1804,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1812,7 +1823,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1831,7 +1842,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1850,7 +1861,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1869,7 +1880,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1888,7 +1899,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1907,7 +1918,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1926,7 +1937,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1945,7 +1956,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1964,7 +1975,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1983,7 +1994,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2002,7 +2013,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2021,7 +2032,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2040,7 +2051,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2059,7 +2070,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2078,7 +2089,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2097,7 +2108,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2116,7 +2127,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2135,7 +2146,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Abner Jimenez.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git2021\ProyectoFinal_SneakersShop\ProyectoFinal_SneakersShoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A54D9FC-34B3-4E86-B19E-EEA645B7E361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9580A1C-C2D0-4D38-BB03-7E611266A739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Programador #9: Diagrama Entidad Relación</t>
+  </si>
+  <si>
+    <t>Abner Nehemias Jimenez Morales</t>
+  </si>
+  <si>
+    <t>Programador #10</t>
   </si>
 </sst>
 </file>
@@ -354,7 +360,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -363,13 +370,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -393,16 +406,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,12 +726,12 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="I16" sqref="I16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -744,47 +750,47 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -803,267 +809,271 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="17" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="16" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="16" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="16" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="16" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="16" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="19"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="5"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="16" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
+      <c r="E16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1082,7 +1092,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1101,7 +1111,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1120,7 +1130,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1139,7 +1149,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1158,7 +1168,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1177,7 +1187,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1196,7 +1206,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1215,7 +1225,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1234,7 +1244,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1253,7 +1263,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1272,7 +1282,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1291,7 +1301,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1310,7 +1320,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1329,7 +1339,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1348,7 +1358,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1367,7 +1377,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1386,7 +1396,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1405,7 +1415,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1424,7 +1434,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1443,7 +1453,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1462,7 +1472,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1481,7 +1491,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1500,7 +1510,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1519,7 +1529,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1538,7 +1548,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1557,7 +1567,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1576,7 +1586,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1595,7 +1605,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1614,7 +1624,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1633,7 +1643,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1652,7 +1662,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1671,7 +1681,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1690,7 +1700,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1709,7 +1719,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1728,7 +1738,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1747,7 +1757,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1766,7 +1776,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1785,7 +1795,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1804,7 +1814,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1823,7 +1833,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1842,7 +1852,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1861,7 +1871,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1880,7 +1890,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1899,7 +1909,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1918,7 +1928,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1937,7 +1947,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1956,7 +1966,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1975,7 +1985,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1994,7 +2004,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2013,7 +2023,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2032,7 +2042,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2051,7 +2061,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2070,7 +2080,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2089,7 +2099,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2108,7 +2118,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2127,7 +2137,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2146,7 +2156,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2167,15 +2177,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E2:L3"/>
@@ -2192,6 +2193,15 @@
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Diego Coyote.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coyot\Documents\GitHub\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1E847D-9EDF-4CDA-9DDA-59DBE5EB761B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31786494-4FA2-4D47-A38A-7E8A0AE63BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -132,34 +132,6 @@
         <rFont val="Century Gothic"/>
         <family val="2"/>
       </rPr>
-      <t>Scrum Master</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Organización en Trello</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF002060"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
       <t>Programador #9</t>
     </r>
     <r>
@@ -189,6 +161,15 @@
   </si>
   <si>
     <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Scrum Master: Organización en Trello</t>
+  </si>
+  <si>
+    <t>Diego Issaac Coyote Sincal</t>
+  </si>
+  <si>
+    <t>Programador #7</t>
   </si>
 </sst>
 </file>
@@ -562,19 +543,38 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,9 +593,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,22 +622,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,13 +650,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>302558</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>464997</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>112060</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1014,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B787FD3E-E662-4E35-B039-84FCC183982F}">
-  <dimension ref="A1:S78"/>
+  <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,11 +1053,11 @@
     </row>
     <row r="3" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
+      <c r="B3" s="18" t="s">
+        <v>17</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1098,16 +1079,16 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1121,14 +1102,14 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1142,18 +1123,18 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33" t="s">
-        <v>20</v>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15" t="s">
+        <v>19</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1184,10 +1165,10 @@
       <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1209,18 +1190,18 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="25" t="s">
-        <v>19</v>
+      <c r="E9" s="31" t="s">
+        <v>18</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1234,18 +1215,18 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1259,18 +1240,18 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="16" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1284,18 +1265,18 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="16" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1309,18 +1290,18 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="16" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1334,18 +1315,18 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="10" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1359,16 +1340,16 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="12"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="N15" s="5"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -1380,20 +1361,20 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="19" t="s">
-        <v>9</v>
+      <c r="E16" s="9" t="s">
+        <v>21</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10" t="s">
-        <v>16</v>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="5"/>
+      <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -1403,16 +1384,20 @@
     <row r="17" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="12"/>
+      <c r="E17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1424,16 +1409,20 @@
     <row r="18" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12"/>
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1442,23 +1431,23 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="19" t="s">
-        <v>10</v>
+      <c r="E19" s="26" t="s">
+        <v>11</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="10" t="s">
-        <v>17</v>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="22"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1467,23 +1456,19 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2039,25 +2024,23 @@
       <c r="S46" s="4"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -2629,30 +2612,27 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="26">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E4:L5"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="I6:L6"/>
@@ -2660,24 +2640,6 @@
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="E13:H13"/>
     <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E4:L5"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="E10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó nombre y puesto de trabajo de Wilmer Chajón.
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1E847D-9EDF-4CDA-9DDA-59DBE5EB761B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4105367B-FFD9-43C9-8AB9-07421896A889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Sneakers Shoes</t>
   </si>
@@ -190,12 +189,18 @@
   <si>
     <t>Scrum Master</t>
   </si>
+  <si>
+    <t>Wilmer Adolfo Chajón Monroy</t>
+  </si>
+  <si>
+    <t>Programador #6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +273,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -551,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -562,19 +573,38 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,9 +623,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,22 +652,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1013,11 +1027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B787FD3E-E662-4E35-B039-84FCC183982F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="I15" sqref="I15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,11 +1086,11 @@
     </row>
     <row r="3" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1098,16 +1112,16 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1121,14 +1135,14 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1142,18 +1156,18 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1184,10 +1198,10 @@
       <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1209,18 +1223,18 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1234,18 +1248,18 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1259,18 +1273,18 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="16" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1284,18 +1298,18 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="16" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1309,18 +1323,18 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="16" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1334,18 +1348,18 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="10" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1359,14 +1373,18 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="12"/>
+      <c r="E15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1380,18 +1398,18 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="4"/>
@@ -1405,14 +1423,14 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="12"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1426,14 +1444,14 @@
       <c r="B18" s="3"/>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1447,18 +1465,18 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="10" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1472,18 +1490,18 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="13" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2650,18 +2668,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="E15:H15"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I18:L18"/>
@@ -2678,6 +2684,18 @@
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="I9:L9"/>
     <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="E15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualizó Datos_de_Programadores.xlsx .
</commit_message>
<xml_diff>
--- a/Datos_de_Programadores.xlsx
+++ b/Datos_de_Programadores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coyot\Documents\GitHub\ProyectoFinal_SneakersShoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProyectoFinal_SneakersShoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C71880-0018-4BC7-9C48-DA43AF3F1A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540F2A12-EB42-4737-8C27-5CA3A12CC1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Alvaro Ramiro Alburez Rivera</t>
-  </si>
-  <si>
-    <t>Progamador#2</t>
   </si>
   <si>
     <t>Josue Daniel Alvarado Cabrera</t>
@@ -67,34 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">Puesto | Actividad </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF002060"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>Progamador #1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Base de datos </t>
-    </r>
   </si>
   <si>
     <r>
@@ -176,6 +145,37 @@
   </si>
   <si>
     <t>Programador #7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Programador #1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Base de datos </t>
+    </r>
+  </si>
+  <si>
+    <t>Programador#2</t>
   </si>
 </sst>
 </file>
@@ -556,33 +556,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -590,6 +563,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,6 +587,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -635,6 +617,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -702,6 +702,61 @@
         <a:xfrm>
           <a:off x="302558" y="6174441"/>
           <a:ext cx="3400939" cy="1411943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238989</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>379203</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B635FC7-A94F-4341-A998-7FFE0E3C6FBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="000000"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="000000">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11373971" y="235324"/>
+          <a:ext cx="2681871" cy="2922938"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1012,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,11 +1123,11 @@
     </row>
     <row r="3" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="18" t="s">
-        <v>17</v>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1094,16 +1149,16 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1117,14 +1172,14 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1138,18 +1193,18 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="15" t="s">
-        <v>9</v>
+      <c r="E6" s="33" t="s">
+        <v>8</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="15" t="s">
-        <v>19</v>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="33" t="s">
+        <v>17</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1205,18 +1260,18 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="32" t="s">
-        <v>18</v>
+      <c r="E9" s="26" t="s">
+        <v>16</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="32" t="s">
-        <v>13</v>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="26" t="s">
+        <v>12</v>
       </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="34"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1230,18 +1285,18 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="12" t="s">
-        <v>14</v>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32" t="s">
+        <v>23</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1255,18 +1310,18 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="24" t="s">
-        <v>3</v>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="17" t="s">
+        <v>24</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="19"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1280,18 +1335,18 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="26"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1305,18 +1360,18 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="26"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1330,18 +1385,18 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="9" t="s">
-        <v>8</v>
+      <c r="E14" s="20" t="s">
+        <v>7</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="20" t="s">
-        <v>15</v>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="11" t="s">
+        <v>13</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1355,18 +1410,18 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="9" t="s">
-        <v>20</v>
+      <c r="E15" s="20" t="s">
+        <v>18</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="17" t="s">
-        <v>21</v>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="35" t="s">
+        <v>19</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1380,18 +1435,18 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="9" t="s">
-        <v>23</v>
+      <c r="E16" s="20" t="s">
+        <v>21</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="24" t="s">
-        <v>24</v>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="4"/>
@@ -1405,18 +1460,18 @@
       <c r="B17" s="3"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="9" t="s">
-        <v>9</v>
+      <c r="E17" s="20" t="s">
+        <v>8</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="20" t="s">
-        <v>22</v>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="11" t="s">
+        <v>20</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1430,18 +1485,18 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="9" t="s">
-        <v>10</v>
+      <c r="E18" s="20" t="s">
+        <v>9</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="20" t="s">
-        <v>16</v>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="11" t="s">
+        <v>14</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1455,18 +1510,18 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="23"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -2633,6 +2688,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="E15:H15"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I18:L18"/>
@@ -2649,16 +2714,6 @@
     <mergeCell ref="I9:L9"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="E15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>